<commit_message>
Frontend avance 1 de enero
</commit_message>
<xml_diff>
--- a/controllers/files/Calendario Plantilla.xlsx
+++ b/controllers/files/Calendario Plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Residencia\Archivos Para Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C56F91A-D4AB-4152-A840-3719201ACAC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFB753E-46FB-4D1B-87AF-7AEFC8F578EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" tabRatio="906" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -569,82 +569,82 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="8" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="8" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Millares 12" xfId="9" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -736,7 +736,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>881707</xdr:colOff>
+      <xdr:colOff>439747</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>121748</xdr:rowOff>
     </xdr:to>
@@ -1048,8 +1048,8 @@
   </sheetPr>
   <dimension ref="B1:AD45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1062,94 +1062,94 @@
     <col min="6" max="6" width="15.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.44140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.44140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15.77734375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5546875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="13.6640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="14.33203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="17.44140625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.21875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.21875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="19" style="1" customWidth="1"/>
+    <col min="16" max="16" width="18.44140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="19.33203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="18.109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.88671875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="20.33203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5546875" style="1" customWidth="1"/>
     <col min="22" max="22" width="9" style="1" customWidth="1"/>
     <col min="23" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:30" s="3" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
     </row>
     <row r="2" spans="2:30" s="3" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="41"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="45"/>
     </row>
     <row r="3" spans="2:30" s="3" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
-      <c r="T3" s="41"/>
-      <c r="U3" s="41"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="45"/>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="45"/>
+      <c r="R3" s="45"/>
+      <c r="S3" s="45"/>
+      <c r="T3" s="45"/>
+      <c r="U3" s="45"/>
     </row>
     <row r="4" spans="2:30" s="3" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:30" s="3" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
@@ -1158,72 +1158,72 @@
         <v>5</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="L6" s="43" t="s">
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="L6" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="44"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="49"/>
       <c r="T6" s="1"/>
     </row>
     <row r="7" spans="2:30" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="43" t="s">
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="48"/>
-      <c r="P7" s="49"/>
-      <c r="Q7" s="49"/>
-      <c r="R7" s="49"/>
-      <c r="S7" s="49"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="53"/>
+      <c r="Q7" s="53"/>
+      <c r="R7" s="53"/>
+      <c r="S7" s="53"/>
       <c r="T7" s="4"/>
     </row>
     <row r="8" spans="2:30" s="3" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="46"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="L8" s="46" t="s">
+      <c r="B8" s="50"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="L8" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="46"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="49"/>
-      <c r="Q8" s="49"/>
-      <c r="R8" s="49"/>
-      <c r="S8" s="49"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="53"/>
+      <c r="Q8" s="53"/>
+      <c r="R8" s="53"/>
+      <c r="S8" s="53"/>
       <c r="T8" s="5"/>
     </row>
     <row r="9" spans="2:30" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1231,44 +1231,44 @@
         <v>9</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="50"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
+      <c r="E9" s="54"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
       <c r="L9" s="2"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="52"/>
-      <c r="S9" s="52"/>
-      <c r="T9" s="52"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="56"/>
+      <c r="S9" s="56"/>
+      <c r="T9" s="56"/>
     </row>
     <row r="10" spans="2:30" s="3" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
       <c r="L10" s="2"/>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
-      <c r="Q10" s="52"/>
-      <c r="R10" s="52"/>
-      <c r="S10" s="52"/>
-      <c r="T10" s="52"/>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="56"/>
+      <c r="S10" s="56"/>
+      <c r="T10" s="56"/>
       <c r="AC10" s="8"/>
       <c r="AD10" s="8"/>
     </row>
@@ -1298,12 +1298,12 @@
       <c r="U12" s="9"/>
     </row>
     <row r="13" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="55"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="60" t="s">
+      <c r="C13" s="62"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="67" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="11" t="s">
@@ -1328,10 +1328,10 @@
       <c r="U13" s="14"/>
     </row>
     <row r="14" spans="2:30" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="57"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="61"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="68"/>
       <c r="F14" s="15" t="s">
         <v>14</v>
       </c>
@@ -1382,7 +1382,7 @@
       </c>
     </row>
     <row r="15" spans="2:30" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B15" s="67"/>
+      <c r="B15" s="43"/>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15" s="37"/>
@@ -1401,10 +1401,10 @@
       <c r="R15" s="34"/>
       <c r="S15" s="18"/>
       <c r="T15" s="18"/>
-      <c r="U15" s="68"/>
+      <c r="U15" s="44"/>
     </row>
     <row r="16" spans="2:30" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="65"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="39"/>
       <c r="D16" s="40"/>
       <c r="E16" s="38"/>
@@ -1423,7 +1423,7 @@
       <c r="R16" s="32"/>
       <c r="S16" s="33"/>
       <c r="T16" s="33"/>
-      <c r="U16" s="66"/>
+      <c r="U16" s="42"/>
     </row>
     <row r="17" spans="2:22" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17"/>
@@ -1963,11 +1963,11 @@
       <c r="V40"/>
     </row>
     <row r="41" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B41" s="64"/>
-      <c r="C41" s="64"/>
-      <c r="D41" s="64"/>
-      <c r="E41" s="64"/>
-      <c r="F41" s="64"/>
+      <c r="B41" s="60"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
     </row>
     <row r="42" spans="2:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C42" s="30"/>
@@ -1979,18 +1979,18 @@
       <c r="C43" s="30"/>
     </row>
     <row r="44" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="62"/>
-      <c r="C44" s="62"/>
-      <c r="D44" s="62"/>
-      <c r="E44" s="62"/>
-      <c r="F44" s="62"/>
+      <c r="B44" s="58"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="58"/>
+      <c r="E44" s="58"/>
+      <c r="F44" s="58"/>
     </row>
     <row r="45" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B45" s="63"/>
-      <c r="C45" s="63"/>
-      <c r="D45" s="63"/>
-      <c r="E45" s="63"/>
-      <c r="F45" s="63"/>
+      <c r="B45" s="59"/>
+      <c r="C45" s="59"/>
+      <c r="D45" s="59"/>
+      <c r="E45" s="59"/>
+      <c r="F45" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -2021,7 +2021,7 @@
     <mergeCell ref="O6:S6"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.19685039370078741" top="0.31496062992125984" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="47" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="38" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>